<commit_message>
updated edges.py and the input files
</commit_message>
<xml_diff>
--- a/continuing.xlsx
+++ b/continuing.xlsx
@@ -5615,37 +5615,37 @@
     <t xml:space="preserve">I am a face-to-face type of person and would like to interact with my fresher buddies physically. I hope they really love sports too so I could show them some moves on the court or field whilst spending a good time with them.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ghana, United States, United Kingdom</t>
+    <t xml:space="preserve">Ghana,United States,United Kingdom</t>
   </si>
   <si>
     <t xml:space="preserve">Cameroonain</t>
   </si>
   <si>
-    <t xml:space="preserve">South Africa, Kenya, Uganda, Ghana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghana, Cameroon, Kenya </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghana, Nigeria, Cameroon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghana, Nigeria, Rwanda, Kenya,Tanzania </t>
+    <t xml:space="preserve">South Africa,Kenya,Uganda,Ghana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghana,Cameroon,Kenya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghana, Nigeria,Cameroon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghana,Nigeria,Rwanda,Kenya,Tanzania </t>
   </si>
   <si>
     <t xml:space="preserve">Not Ghana</t>
   </si>
   <si>
-    <t xml:space="preserve">Rwanda, Cameroon, Zimbabwe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghana, Cameroon, Kenya, Ivory Coast</t>
+    <t xml:space="preserve">Rwanda,Cameroon,Zimbabwe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghana,Cameroon,Kenya,Ivory Coast</t>
   </si>
   <si>
     <t xml:space="preserve">Congolese</t>
   </si>
   <si>
-    <t xml:space="preserve">Cameroon, Rwanda </t>
+    <t xml:space="preserve">Cameroon,Rwanda </t>
   </si>
   <si>
     <t xml:space="preserve">Ghana, United Kingdom, United States</t>
@@ -16770,7 +16770,7 @@
   <dimension ref="A1:I178"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16778,7 +16778,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="79.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20"/>
   </cols>
   <sheetData>
@@ -17236,7 +17236,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>37</v>

</xml_diff>